<commit_message>
1. ImportPhrasesFile -> data return list of dictionaries
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -1,67 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\konshinav\st\python\eng_simulator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A200C291-A30D-4779-AEE2-F91B6E3B5390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Phrases" sheetId="1" r:id="rId1"/>
+    <sheet name="Phrases" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>En</t>
-  </si>
-  <si>
-    <t>Ru</t>
-  </si>
-  <si>
-    <t>dog</t>
-  </si>
-  <si>
-    <t>cat</t>
-  </si>
-  <si>
-    <t>кошка</t>
-  </si>
-  <si>
-    <t>собак</t>
-  </si>
-  <si>
-    <t>bird</t>
-  </si>
-  <si>
-    <t>птица</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -80,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -382,45 +408,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>En</t>
+        </is>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Ru</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Check for add dublicates
add "date_last_attemmt DATETIME"
set en_value, ru_value (SQL) as UNIQUE
add method "import_phrases_into_module" to class "lesson"
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -1,40 +1,441 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\konshinav\st\python\eng_simulator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC26FE5-EF83-4DC5-8B06-C42C8B1B7303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Phrases" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Phrases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>En</t>
+  </si>
+  <si>
+    <t>Ru</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I would like to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">point out </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">that it’s </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">extremely </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>important</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Я бы хотел </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>заметить</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, что это </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>чрезвычайно</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> важно</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I’d like to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">point out </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>that it isn’t enough</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Я хотел бы </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>заметить</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>что этого не достаточно</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Let me </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">point out </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">that we can’t </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">achieve success </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>without hard work</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Позволь мне </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">заметить </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">что, мы не можем </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">достичь успеха </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>без усердной работы</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I want to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">point out </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">that success </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>can’t be achieved</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> without hard work</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Я хочу </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">заметить </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">что, успех </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">не может быть достигнут </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>без усердной работы</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I like to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">point out </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>that it is not enough to get this level</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Я хотел бы </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>заметить</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> что, этого недостаточно чтобы получить этот уровень</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <scheme val="minor"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,85 +443,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,32 +768,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.5703125" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>En</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Ru</t>
-        </is>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>